<commit_message>
some of the functionalities work, reveals the correct character, deducts from remaining if wrong, but duplicate is still an issue
</commit_message>
<xml_diff>
--- a/plot.xlsx
+++ b/plot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>JS</t>
   </si>
@@ -92,21 +92,6 @@
     <t>arrImage</t>
   </si>
   <si>
-    <t>cpuName</t>
-  </si>
-  <si>
-    <t>remaining</t>
-  </si>
-  <si>
-    <t>usedLetters</t>
-  </si>
-  <si>
-    <t>counterW</t>
-  </si>
-  <si>
-    <t>counterL</t>
-  </si>
-  <si>
     <t>Array</t>
   </si>
   <si>
@@ -122,34 +107,133 @@
     <t>Names</t>
   </si>
   <si>
-    <t>Arya Stark</t>
-  </si>
-  <si>
-    <t>Bran Stark</t>
-  </si>
-  <si>
-    <t>Cersei Lannister</t>
-  </si>
-  <si>
-    <t>Daenerys Targaryen</t>
-  </si>
-  <si>
-    <t>Jamie Lannister</t>
-  </si>
-  <si>
-    <t>Jon Snow</t>
-  </si>
-  <si>
-    <t>Jorah Mormont</t>
-  </si>
-  <si>
-    <t>Sansa Stark</t>
-  </si>
-  <si>
-    <t>Theon Greyjoy</t>
-  </si>
-  <si>
-    <t>Tyrion Lannister</t>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>set play to "True"</t>
+  </si>
+  <si>
+    <t>select a character</t>
+  </si>
+  <si>
+    <t>update currentWord with blanks</t>
+  </si>
+  <si>
+    <t>set remaining gusses to 12</t>
+  </si>
+  <si>
+    <t>update wins</t>
+  </si>
+  <si>
+    <t>update loses</t>
+  </si>
+  <si>
+    <t>clear guessed letters</t>
+  </si>
+  <si>
+    <t>hide instructions</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>arrGuessedLetters</t>
+  </si>
+  <si>
+    <t>strCpuName</t>
+  </si>
+  <si>
+    <t>arrCpuName</t>
+  </si>
+  <si>
+    <t>strpuImage</t>
+  </si>
+  <si>
+    <t>intRemaining</t>
+  </si>
+  <si>
+    <t>arrUsedLetters</t>
+  </si>
+  <si>
+    <t>intCounterW</t>
+  </si>
+  <si>
+    <t>intCounterL</t>
+  </si>
+  <si>
+    <t>bolPlay</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Arya</t>
+  </si>
+  <si>
+    <t>Bran</t>
+  </si>
+  <si>
+    <t>Cately</t>
+  </si>
+  <si>
+    <t>Cersei</t>
+  </si>
+  <si>
+    <t>Daenerys</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Joffrey</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Sansa</t>
+  </si>
+  <si>
+    <t>Tyrion</t>
+  </si>
+  <si>
+    <t>Lannister</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Baratheon</t>
+  </si>
+  <si>
+    <t>Targaryen</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>if key doesn't match any of the letters in the name</t>
+  </si>
+  <si>
+    <t>if key matches any of the letters in the name</t>
+  </si>
+  <si>
+    <t>reveal the letter</t>
+  </si>
+  <si>
+    <t>add letter to guessed letters</t>
+  </si>
+  <si>
+    <t>Checker</t>
   </si>
 </sst>
 </file>
@@ -213,9 +297,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -496,237 +582,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="27.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="1" max="16384" width="27.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="str">
+        <f>C29&amp;" "&amp;D29</f>
+        <v>Arya Stark</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="str">
+        <f t="shared" ref="B30:B38" si="0">C30&amp;" "&amp;D30</f>
+        <v>Bran Stark</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Cately Stark</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Cersei Lannister</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Daenerys Targaryen</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Jaime Lannister</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Joffrey Baratheon</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Jon Snow</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sansa Stark</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Tyrion Lannister</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
-        <v>40</v>
+    <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>